<commit_message>
refinements - ready to merge geocodes
</commit_message>
<xml_diff>
--- a/data/1963-2024 HHT Homeowners_Adresses.xlsx
+++ b/data/1963-2024 HHT Homeowners_Adresses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-24.04\home\john\projects\ssg-thefan-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFD9A86-CAA3-42A8-AA0E-80D9F0153706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FEECB2-A77A-4ACF-8A6D-8A78DF04A8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4968" yWindow="2748" windowWidth="23040" windowHeight="13560" xr2:uid="{B5D97D05-3EDC-47CB-BC1F-7CDFD2452C40}"/>
+    <workbookView xWindow="5508" yWindow="1164" windowWidth="23040" windowHeight="13560" xr2:uid="{B5D97D05-3EDC-47CB-BC1F-7CDFD2452C40}"/>
   </bookViews>
   <sheets>
     <sheet name="1963-2024" sheetId="2" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t xml:space="preserve">1803 Hanover Ave.– Mr. &amp; Mrs. George (Judith) Booker III  </t>
   </si>
   <si>
-    <t xml:space="preserve">1900 Hanover Ave.– Honorable &amp; Mrs. Fred (Jane)Pollard  </t>
-  </si>
-  <si>
     <t xml:space="preserve">1719 Park Ave.– Mr. &amp; Mrs. David (Carlyle) Clinger  </t>
   </si>
   <si>
@@ -351,12 +348,6 @@
     <t xml:space="preserve">2021 Stuart Ave. – Dr. &amp; Mrs. Bennett (Susan) Malbon   </t>
   </si>
   <si>
-    <t xml:space="preserve">St. John’s United Church of Christ  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">605-12 N. Davis – Mr. David E. Martin  </t>
-  </si>
-  <si>
     <r>
       <t>1973</t>
     </r>
@@ -543,9 +534,6 @@
     <t xml:space="preserve">Tour B  </t>
   </si>
   <si>
-    <t xml:space="preserve">2500 ½ Kensington Ave. – Mr. George Ruark   </t>
-  </si>
-  <si>
     <r>
       <t>2509</t>
     </r>
@@ -624,9 +612,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">402 N. Allen Ave. – Mr. &amp; Mrs. William (Regena) Carreras  </t>
-  </si>
-  <si>
     <t xml:space="preserve">1707 Grove Ave. – Mr. &amp; Mrs. Drew St. J. (Anne) Carneal  </t>
   </si>
   <si>
@@ -715,12 +700,6 @@
     <t xml:space="preserve">1419 Park Ave. - Mr. Stuart Siegel  </t>
   </si>
   <si>
-    <t xml:space="preserve">500 N. Allen Ave. -- The Martin Agency  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">605 N. Davis (Ingleside Ct.) -- Mr. J. Clarke Plaxco  </t>
-  </si>
-  <si>
     <t xml:space="preserve">1607 Floyd Ave. – Mr. &amp; Mrs. Bruce (Patronella) Tyler  </t>
   </si>
   <si>
@@ -756,15 +735,6 @@
     <t xml:space="preserve">1916 Floyd Ave., Mr. &amp; Mrs. Bob (Noretta) Taylor   </t>
   </si>
   <si>
-    <t xml:space="preserve">821 W. Franklin Ave., Ritter Hickok House, VCU  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">901 W. Franklin Ave., Ginter House, VCU  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">910 W. Franklin Ave., The President’s House, VCU  </t>
-  </si>
-  <si>
     <t xml:space="preserve">1308 Grove Ave., Dr. Waverly M. Cole &amp; Mr. John Cook  </t>
   </si>
   <si>
@@ -795,9 +765,6 @@
       </rPr>
       <t xml:space="preserve">- Chair, Mr. James Corum  </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">1800 West Grace St. -- Virginia Auto Dealers Association  </t>
   </si>
   <si>
     <t xml:space="preserve">1505 Hanover Ave. – Mr. &amp; Mrs. Charles (May) Fox   </t>
@@ -851,9 +818,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">1400 Floyd Ave. (The Warsaw) -- Mr. &amp; Mrs. Overton Dennis  </t>
-  </si>
-  <si>
     <t xml:space="preserve">2206 Floyd Ave. -- Mr. Ronnie Drake  </t>
   </si>
   <si>
@@ -889,18 +853,12 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">402 N. Allen – Mr. &amp; Mrs. William (Regina) Carreras Grace at Lombardy – The Columbia   </t>
-  </si>
-  <si>
     <t xml:space="preserve">1823 Hanover Ave – Mr. Michael Krumbein &amp; Ms. Jane Keyser  </t>
   </si>
   <si>
     <t xml:space="preserve">1700 Hanover Ave. – Mr. John Adair  </t>
   </si>
   <si>
-    <t xml:space="preserve">2235 Monument Ave., #3 (Rixey Court) – Mr. &amp; Mrs. G. William (Marie) White, Jr.  </t>
-  </si>
-  <si>
     <t xml:space="preserve">2340 Monument Ave. – Dr. &amp; Mrs. Gerasim (Edith) Tikoff  </t>
   </si>
   <si>
@@ -928,15 +886,6 @@
   </si>
   <si>
     <t xml:space="preserve">1504 Floyd Ave. – Mr. &amp; Mrs. Bill (Susan) Grove  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1506 W. Main St. – Mr. &amp; Mrs. Jim (Penny) Stygar (Folio 2, Inc.)  </t>
-  </si>
-  <si>
-    <t>1514 W. Main St. -- Reynolds/Minor Gallery, Beverly Reynolds &amp;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charlotte Minor 2503 Kensington Ave. – Ms.  Dottie Smith  </t>
   </si>
   <si>
     <t xml:space="preserve">2610 Monument Ave. – Mr. &amp; Mrs. Richard (Sylvia) Summers  </t>
@@ -1176,15 +1125,6 @@
     <t xml:space="preserve">1519 Hanover Ave. – Mr. Vernon Smith  </t>
   </si>
   <si>
-    <t xml:space="preserve">507 N. Lombardy St. (St. John’s United Church of Christ)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1603 Monument Ave (First Lutheran Church)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1627 Monument Ave. (Grace Covenant Presbyterian Church)  </t>
-  </si>
-  <si>
     <t xml:space="preserve">1516 Park Ave. – Mr. Charles J. Cooper  </t>
   </si>
   <si>
@@ -1327,9 +1267,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">402 N. Allen Ave. – Mr. &amp; Mrs. William (Rejena) Carreras  </t>
-  </si>
-  <si>
     <t xml:space="preserve">405 N. Allen Ave. – Mr. &amp; Mrs. Dick (Nancy) Krider  </t>
   </si>
   <si>
@@ -1630,9 +1567,6 @@
     <t xml:space="preserve">2326 Monument Ave. – Ms. Tina Baccus &amp; Mr. Warren Frye  </t>
   </si>
   <si>
-    <t xml:space="preserve">2501 Monument Ave. -- Branch House  </t>
-  </si>
-  <si>
     <t xml:space="preserve">2516 Monument Ave. – Mr. Clay Hamner  </t>
   </si>
   <si>
@@ -1713,9 +1647,6 @@
   </si>
   <si>
     <t xml:space="preserve">2024 Hanover Ave. – Mr. Ray Ashworth  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1627 Monument Ave. – Grace Covenant Presbyterian Church  </t>
   </si>
   <si>
     <t xml:space="preserve">1530 Park Ave. – Mr. Abby W. Moore  </t>
@@ -1843,9 +1774,6 @@
     <t xml:space="preserve">2200 Stuart Ave. – Mr. David Worstine  </t>
   </si>
   <si>
-    <t xml:space="preserve">2200A Stuart Ave. – Mr. Irving Schiff  </t>
-  </si>
-  <si>
     <t xml:space="preserve">2409 Stuart Ave. – Mr. &amp; Mrs. Ed (Rosalie) Lowman  </t>
   </si>
   <si>
@@ -1887,9 +1815,6 @@
     <t xml:space="preserve">1015 W. Franklin St.– Mr. David van Blaricom &amp; Ms. Kelly Taylor  </t>
   </si>
   <si>
-    <t xml:space="preserve">314 N. Harrison – Ms. Linda Heavenridge &amp; Mr. Ed Parker  </t>
-  </si>
-  <si>
     <t xml:space="preserve">208 N. Plum St. – Ms. Jane Brooke  </t>
   </si>
   <si>
@@ -2071,9 +1996,6 @@
   </si>
   <si>
     <t xml:space="preserve">1508 Grove Ave. – Mr. &amp; Mrs. Austin (Trudi) Mehrhof  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">312 N. Harrison St. – Ms. Margaret Traylor One Monument Ave   </t>
   </si>
   <si>
     <t xml:space="preserve">1104 West Ave. – Mr. Theodore Adams  </t>
@@ -2283,9 +2205,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">1652 W. Grace St., #2A – Ms. Kathleen Barrett  </t>
-  </si>
-  <si>
     <t xml:space="preserve">310 N. Granby St. – Mr. Michael Mayberry  </t>
   </si>
   <si>
@@ -2301,9 +2220,6 @@
     <t xml:space="preserve">1708 Hanover Ave. – Mr. &amp; Mrs. Jerome (Gail) Beverage  </t>
   </si>
   <si>
-    <t xml:space="preserve">1723 Hanover Ave., #4 – Ms. Patricia Bryant  </t>
-  </si>
-  <si>
     <t xml:space="preserve">1837 Monument Ave. – Ms. Natalie Ellis  </t>
   </si>
   <si>
@@ -2404,15 +2320,9 @@
     <t xml:space="preserve">1612 Park Ave. – Mr. Gene Ramey &amp; Mr. Don Thompson  </t>
   </si>
   <si>
-    <t xml:space="preserve">1723 Hanover Ave., #7 – Mr. &amp; Mrs. Doc (Pat) Outland  </t>
-  </si>
-  <si>
     <t xml:space="preserve">2226 Park Ave. – Ms. Jacqueline Brophy &amp; Mr. Lenny Wheeler  </t>
   </si>
   <si>
-    <t xml:space="preserve">1901 Stuart Ave., #1, Mr. &amp; Mrs. Bob (Barb) Dittmeier  </t>
-  </si>
-  <si>
     <t xml:space="preserve">2020 Stuart Ave. -- Mr. Robert Rentz   </t>
   </si>
   <si>
@@ -2593,9 +2503,6 @@
   </si>
   <si>
     <t>112 Harvie St – Ms. Ann Woods Cutchins</t>
-  </si>
-  <si>
-    <t>Appliance House, 823 Broad Street – Ms. Candy Osdene</t>
   </si>
   <si>
     <t>819 Broad Street – Ms. Renate Forssmann-Falk</t>
@@ -3019,9 +2926,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">2625 Monument Ave., Mr. &amp; Mrs. John (Carolyn) Snow   </t>
-  </si>
-  <si>
     <t xml:space="preserve">2402 Park Ave. -- Mr. &amp; Mrs. Stafford (Shirley) White   </t>
   </si>
   <si>
@@ -3032,9 +2936,6 @@
   </si>
   <si>
     <t xml:space="preserve">2005 W. Grace St. -- Mr. &amp; Mrs. Thomas E. Machia  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2501 Monument Ave. – Branch House (offices of Virginia agency of Northwestern Mutual Life)  </t>
   </si>
   <si>
     <t xml:space="preserve">2704 Monument Ave. – Mr. &amp; Mrs. Donald P. (Dorothy) Irwin </t>
@@ -3217,12 +3118,6 @@
     <t>1825 Grove Ave – Ms. Kate Ogden</t>
   </si>
   <si>
-    <t>2330 Monument Ave - The Ronald McDonald House</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tryme Gallery, 1623 Main Street - Mr. &amp; Mrs. Bill (Pam) Royall </t>
-  </si>
-  <si>
     <t>2336 Monument Ave - Mr. &amp; Mrs. Bill (Ceci) Gallasch</t>
   </si>
   <si>
@@ -3317,9 +3212,6 @@
   </si>
   <si>
     <t xml:space="preserve">1910 Grove Ave. – Mr. &amp; Mrs. George (Jo) Kennedy  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2225 Hanover Ave. -- Fan Poster Gallery  </t>
   </si>
   <si>
     <t xml:space="preserve">418 N. Stafford St. – Mr. Carey Lindsey   </t>
@@ -3348,9 +3240,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">2330 Monument Ave. -- Ronald McDonald House   </t>
-  </si>
-  <si>
     <t xml:space="preserve">1530 Park Ave. – Mr. Michael B. Wray </t>
   </si>
   <si>
@@ -3439,9 +3328,6 @@
     </r>
   </si>
   <si>
-    <t>2501 Monument Avenue - The Branch Museum</t>
-  </si>
-  <si>
     <t>2209 Monument Avenue - Kip Caudle</t>
   </si>
   <si>
@@ -3578,9 +3464,6 @@
     <t>1617 Hanover Avenue - Mary Stuart &amp; Walter Murphy</t>
   </si>
   <si>
-    <t>1423 Floyd Avenue (Warsaw) - Mary &amp; Andy Radford</t>
-  </si>
-  <si>
     <t>1140 West Avenue - Jennifer &amp; Steve Burris</t>
   </si>
   <si>
@@ -3597,9 +3480,6 @@
   </si>
   <si>
     <t>1901 Grove Avenue - Leanne &amp; Alex Kurland</t>
-  </si>
-  <si>
-    <t>1723 Hanover Avenue, Unit 4 - Sharon &amp; John Miller</t>
   </si>
   <si>
     <r>
@@ -3673,9 +3553,6 @@
     <t>2515 Hanover Avenue - Sally &amp; Greg Holzgrefe</t>
   </si>
   <si>
-    <t>1701 Floyd Avenue - Dogwood Middle School</t>
-  </si>
-  <si>
     <t>2306 Floyd Avenue - Pattie &amp; Mike Kennedy</t>
   </si>
   <si>
@@ -3753,6 +3630,129 @@
   </si>
   <si>
     <t>403 N. Allen Ave. - Janet Heltzel &amp; George Hostetler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2503 Kensington Ave. – Ms.  Dottie Smith  </t>
+  </si>
+  <si>
+    <t>1514 W. Main St. -- [Reynolds/Minor Gallery] Beverly Reynolds &amp; Charlotte Minor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1506 W. Main St. – Mr. &amp; Mrs. Jim (Penny) Stygar [Folio 2, Inc.]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2501 Monument Ave. – [Branch House] Offices of Virginia agency of Northwestern Mutual Life  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">402 N. Allen – Mr. &amp; Mrs. William (Regina) Carreras [Columbia House]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2625 Monument Ave. - Mr. &amp; Mrs. John (Carolyn) Snow   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1400 Floyd Ave. [The Warsaw] -- Mr. &amp; Mrs. Overton Dennis  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">605 N. Davis [Ingleside Court] -- Mr. J. Clarke Plaxco  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">402 N. Allen Ave. – Mr. &amp; Mrs. William (Rejena) Carreras [Columbia House]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">402 N. Allen Ave. – Mr. &amp; Mrs. William (Regena) Carreras [Columbia House]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2235 Monument Ave. #3  [Rixey Court] – Mr. &amp; Mrs. G. William (Marie) White, Jr.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">312 N. Harrison St. – Ms. Margaret Traylor [One Monument Ave]   </t>
+  </si>
+  <si>
+    <t>1701 Floyd Avenue - [Dogwood Middle School]</t>
+  </si>
+  <si>
+    <t>2501 Monument Avenue - [Branch House]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2501 Monument Ave. -- [Branch House]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">507 N. Lombardy St. - [St. John’s United Church of Christ]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 507 N. Lombardy St. - [St. John’s United Church of Christ]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1603 Monument Ave - [First Lutheran Church]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1627 Monument Ave. - [Grace Covenant Presbyterian Church]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1627 Monument Ave. – [Grace Covenant Presbyterian Church]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">821 W. Franklin Ave. - [Ritter Hickok House, VCU]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">901 W. Franklin Ave. - [Ginter House, VCU]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">910 W. Franklin Ave. - [The President’s House, VCU]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1800 West Grace St. --[ Virginia Auto Dealers Association]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 N. Allen Ave. -- [The Martin Agency]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2330 Monument Ave. -- [Ronald McDonald House]   </t>
+  </si>
+  <si>
+    <t>2330 Monument Ave - [Ronald McDonald House]</t>
+  </si>
+  <si>
+    <t>823 Broad Street [Appliance House] – Ms. Candy Osdene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1900 Hanover Ave.– Honorable &amp; Mrs. Fred (Jane) Pollard  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500 Kensington Ave. #2 – Mr. George Ruark   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2225 Hanover Ave. -- [Fan Poster Gallery]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2200 #A Stuart Ave. – Mr. Irving Schiff  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1623 Main Street [Tryme Gallery] - Mr. &amp; Mrs. Bill (Pam) Royall </t>
+  </si>
+  <si>
+    <t xml:space="preserve">314 N. Harrison St. – Ms. Linda Heavenridge &amp; Mr. Ed Parker  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1652 W. Grace St. #2A – Ms. Kathleen Barrett  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1723 Hanover Ave. #4 – Ms. Patricia Bryant  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1723 Hanover Ave. #7 – Mr. &amp; Mrs. Doc (Pat) Outland  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1901 Stuart Ave. -- Mr. &amp; Mrs. Bob (Barb) Dittmeier  </t>
+  </si>
+  <si>
+    <t>1723 Hanover Ave. #4 - Sharon &amp; John Miller</t>
+  </si>
+  <si>
+    <t>1423 Floyd Avenue [The Warsaw] - Mary &amp; Andy Radford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">605 N. Davis  #12 [Ingleside Court] – Mr. David E. Martin  </t>
   </si>
 </sst>
 </file>
@@ -4288,8 +4288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82ABAD3-693D-4121-82C0-FE2AABF1CFBD}">
   <dimension ref="A1:D668"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A620" workbookViewId="0">
-      <selection activeCell="A633" sqref="A633"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4300,13 +4300,13 @@
     <row r="1" spans="1:1" ht="96.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:1" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>638</v>
+        <v>597</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>459</v>
+        <v>428</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -4371,22 +4371,22 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>461</v>
+        <v>430</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>538</v>
+        <v>503</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>540</v>
+        <v>505</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>541</v>
+        <v>506</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
@@ -4406,17 +4406,17 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>542</v>
+        <v>507</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>460</v>
+        <v>429</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>543</v>
+        <v>508</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4436,607 +4436,607 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>18</v>
+        <v>629</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>465</v>
+        <v>434</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>539</v>
+        <v>504</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>463</v>
+        <v>432</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>462</v>
+        <v>431</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
-        <v>464</v>
+        <v>433</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>544</v>
+        <v>509</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
-        <v>466</v>
+        <v>435</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
-        <v>468</v>
+        <v>437</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
-        <v>469</v>
+        <v>438</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
-        <v>470</v>
+        <v>439</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
-        <v>51</v>
+        <v>616</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
-        <v>52</v>
+        <v>641</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
-        <v>474</v>
+        <v>443</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
-        <v>471</v>
+        <v>440</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
-        <v>472</v>
+        <v>441</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
-        <v>473</v>
+        <v>442</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
-        <v>475</v>
+        <v>444</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
-        <v>51</v>
+        <v>617</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
-        <v>476</v>
+        <v>445</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
-        <v>477</v>
+        <v>446</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
-        <v>51</v>
+        <v>617</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
-        <v>479</v>
+        <v>448</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
-        <v>478</v>
+        <v>447</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
-        <v>480</v>
+        <v>449</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="109" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
-        <v>75</v>
+        <v>630</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
-        <v>82</v>
+        <v>610</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
-        <v>545</v>
+        <v>510</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
-        <v>546</v>
+        <v>511</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
-        <v>481</v>
+        <v>450</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
-        <v>483</v>
+        <v>452</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
-        <v>482</v>
+        <v>451</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" s="6" t="s">
-        <v>485</v>
+        <v>454</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" s="6" t="s">
-        <v>484</v>
+        <v>453</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="6" t="s">
-        <v>486</v>
+        <v>455</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
-        <v>547</v>
+        <v>512</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="6" t="s">
-        <v>548</v>
+        <v>513</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
-        <v>99</v>
+        <v>625</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="6" t="s">
-        <v>100</v>
+        <v>608</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" s="6" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="6" t="s">
-        <v>549</v>
+        <v>514</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="6" t="s">
-        <v>550</v>
+        <v>631</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
@@ -5046,2591 +5046,2591 @@
     </row>
     <row r="152" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" s="6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="6" t="s">
-        <v>106</v>
+        <v>621</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" s="6" t="s">
-        <v>107</v>
+        <v>622</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="6" t="s">
-        <v>108</v>
+        <v>623</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" s="6" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" s="6" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" s="6" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" s="6" t="s">
-        <v>487</v>
+        <v>456</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="6" t="s">
-        <v>488</v>
+        <v>457</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" s="6" t="s">
-        <v>99</v>
+        <v>625</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" s="6" t="s">
-        <v>113</v>
+        <v>624</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" s="6" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" s="6" t="s">
-        <v>489</v>
+        <v>458</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" s="6" t="s">
-        <v>490</v>
+        <v>459</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" s="6" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" s="6" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" s="6" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" s="6" t="s">
-        <v>491</v>
+        <v>460</v>
       </c>
     </row>
     <row r="173" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="7" t="s">
-        <v>492</v>
+        <v>461</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" s="6" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" s="6" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" s="6" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="6" t="s">
-        <v>494</v>
+        <v>606</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="6" t="s">
-        <v>495</v>
+        <v>463</v>
       </c>
     </row>
     <row r="181" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
-        <v>493</v>
+        <v>462</v>
       </c>
     </row>
     <row r="182" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="6" t="s">
-        <v>124</v>
+        <v>607</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" s="6" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" s="6" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="6" t="s">
-        <v>496</v>
+        <v>464</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="6" t="s">
-        <v>498</v>
+        <v>466</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="6" t="s">
-        <v>497</v>
+        <v>465</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="6" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" s="6" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="191" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A191" s="5" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="6" t="s">
-        <v>130</v>
+        <v>605</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" s="6" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" s="6" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" s="6" t="s">
-        <v>133</v>
+        <v>611</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" s="6" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" s="6" t="s">
-        <v>499</v>
+        <v>604</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" s="6" t="s">
-        <v>500</v>
+        <v>467</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" s="6" t="s">
-        <v>551</v>
+        <v>515</v>
       </c>
     </row>
     <row r="200" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A200" s="5" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" s="6" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202" s="6" t="s">
-        <v>137</v>
+        <v>603</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203" s="6" t="s">
-        <v>138</v>
+        <v>602</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" s="6" t="s">
-        <v>139</v>
+        <v>601</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205" s="6" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206" s="6" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207" s="6" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209" s="6" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
     </row>
     <row r="210" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A210" s="5" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211" s="6" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212" s="6" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213" s="6" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214" s="6" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215" s="6" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216" s="6" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217" s="6" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218" s="6" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219" s="6" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220" s="6" t="s">
-        <v>552</v>
+        <v>516</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221" s="6" t="s">
-        <v>553</v>
+        <v>626</v>
       </c>
     </row>
     <row r="222" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A222" s="5" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223" s="6" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224" s="6" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225" s="6" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" s="6" t="s">
-        <v>159</v>
+        <v>616</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227" s="6" t="s">
-        <v>160</v>
+        <v>618</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228" s="6" t="s">
-        <v>161</v>
+        <v>619</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229" s="6" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230" s="6" t="s">
-        <v>554</v>
+        <v>517</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231" s="6" t="s">
-        <v>525</v>
+        <v>492</v>
       </c>
     </row>
     <row r="232" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A232" s="5" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233" s="6" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234" s="6" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235" s="6" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237" s="6" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238" s="6" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239" s="6" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240" s="6" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241" s="6" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242" s="6" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243" s="6" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244" s="6" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
     </row>
     <row r="245" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A245" s="5" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246" s="6" t="s">
-        <v>176</v>
+        <v>609</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247" s="6" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248" s="6" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249" s="6" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250" s="6" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251" s="6" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252" s="6" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253" s="6" t="s">
-        <v>501</v>
+        <v>468</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254" s="6" t="s">
-        <v>502</v>
+        <v>469</v>
       </c>
     </row>
     <row r="255" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A255" s="5" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256" s="6" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257" s="6" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258" s="6" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259" s="6" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260" s="6" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261" s="6" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262" s="6" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263" s="6" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264" s="6" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265" s="6" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266" s="6" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267" s="6" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268" s="6" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
     </row>
     <row r="269" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="7" t="s">
-        <v>503</v>
+        <v>470</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270" s="6" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271" s="6" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272" s="6" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273" s="6" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274" s="6" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275" s="6" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277" s="6" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278" s="6" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279" s="6" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280" s="6" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281" s="6" t="s">
-        <v>504</v>
+        <v>471</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282" s="6" t="s">
-        <v>505</v>
+        <v>472</v>
       </c>
     </row>
     <row r="283" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A283" s="5" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284" s="6" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285" s="6" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286" s="6" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287" s="6" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288" s="6" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289" s="6" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290" s="6" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291" s="6" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292" s="6" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293" s="6" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
     </row>
     <row r="294" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A294" s="5" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295" s="6" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296" s="6" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297" s="6" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298" s="6" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299" s="6" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300" s="6" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301" s="6" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302" s="6" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303" s="6" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304" s="6" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305" s="6" t="s">
-        <v>506</v>
+        <v>473</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306" s="6" t="s">
-        <v>507</v>
+        <v>474</v>
       </c>
     </row>
     <row r="307" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A307" s="5" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308" s="6" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309" s="6" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310" s="6" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311" s="6" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A312" s="6" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313" s="6" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314" s="6" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315" s="6" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316" s="6" t="s">
-        <v>237</v>
+        <v>615</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317" s="6" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318" s="6" t="s">
-        <v>508</v>
+        <v>475</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319" s="6" t="s">
-        <v>509</v>
+        <v>476</v>
       </c>
     </row>
     <row r="320" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A320" s="5" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321" s="6" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A322" s="6" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A323" s="6" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324" s="6" t="s">
-        <v>243</v>
+        <v>221</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325" s="6" t="s">
-        <v>244</v>
+        <v>222</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326" s="6" t="s">
-        <v>245</v>
+        <v>223</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327" s="6" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A328" s="6" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A329" s="6" t="s">
-        <v>555</v>
+        <v>518</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A330" s="6" t="s">
-        <v>556</v>
+        <v>519</v>
       </c>
     </row>
     <row r="331" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A331" s="5" t="s">
-        <v>248</v>
+        <v>226</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A332" s="6" t="s">
-        <v>249</v>
+        <v>227</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333" s="6" t="s">
-        <v>250</v>
+        <v>228</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A334" s="6" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335" s="6" t="s">
-        <v>252</v>
+        <v>620</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A336" s="6" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337" s="6" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A338" s="6" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A339" s="6" t="s">
-        <v>256</v>
+        <v>233</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A340" s="6" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341" s="6" t="s">
-        <v>639</v>
+        <v>598</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A342" s="6" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
     </row>
     <row r="343" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A343" s="5" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344" s="6" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345" s="6" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A346" s="6" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A347" s="6" t="s">
-        <v>262</v>
+        <v>239</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A348" s="6" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A349" s="6" t="s">
-        <v>264</v>
+        <v>241</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A350" s="6" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A351" s="6" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A352" s="6" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353" s="6" t="s">
-        <v>268</v>
+        <v>632</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A354" s="6" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355" s="6" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
     </row>
     <row r="356" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A356" s="5" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357" s="6" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A358" s="6" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A359" s="6" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A360" s="6" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361" s="6" t="s">
-        <v>510</v>
+        <v>477</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362" s="6" t="s">
-        <v>511</v>
+        <v>478</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A363" s="6" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364" s="6" t="s">
-        <v>276</v>
+        <v>634</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A365" s="6" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A366" s="6" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
     </row>
     <row r="367" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A367" s="5" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A368" s="6" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A369" s="6" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A370" s="6" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A371" s="6" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A372" s="6" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A373" s="6" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A374" s="6" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A375" s="6" t="s">
-        <v>287</v>
+        <v>262</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A376" s="6" t="s">
-        <v>288</v>
+        <v>263</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A377" s="6" t="s">
-        <v>289</v>
+        <v>264</v>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A378" s="6" t="s">
-        <v>290</v>
+        <v>265</v>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A379" s="6" t="s">
-        <v>291</v>
+        <v>266</v>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A380" s="6" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A381" s="6" t="s">
-        <v>293</v>
+        <v>268</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A382" s="6" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
     </row>
     <row r="383" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A383" s="5" t="s">
-        <v>295</v>
+        <v>270</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A384" s="6" t="s">
-        <v>512</v>
+        <v>479</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A385" s="6" t="s">
-        <v>296</v>
+        <v>271</v>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A386" s="6" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387" s="6" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388" s="6" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389" s="6" t="s">
-        <v>300</v>
+        <v>275</v>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A390" s="6" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A391" s="6" t="s">
-        <v>302</v>
+        <v>277</v>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A392" s="6" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393" s="6" t="s">
-        <v>304</v>
+        <v>279</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394" s="6" t="s">
-        <v>305</v>
+        <v>280</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395" s="6" t="s">
-        <v>306</v>
+        <v>281</v>
       </c>
     </row>
     <row r="396" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A396" s="7" t="s">
-        <v>513</v>
+        <v>480</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397" s="6" t="s">
-        <v>307</v>
+        <v>282</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398" s="6" t="s">
-        <v>308</v>
+        <v>283</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399" s="6" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A400" s="6" t="s">
-        <v>309</v>
+        <v>284</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A401" s="6" t="s">
-        <v>310</v>
+        <v>285</v>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A402" s="6" t="s">
-        <v>514</v>
+        <v>481</v>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403" s="6" t="s">
-        <v>515</v>
+        <v>482</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A404" s="6" t="s">
-        <v>311</v>
+        <v>286</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405" s="6" t="s">
-        <v>312</v>
+        <v>287</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A406" s="6" t="s">
-        <v>313</v>
+        <v>288</v>
       </c>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407" s="6" t="s">
-        <v>314</v>
+        <v>289</v>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A408" s="6" t="s">
-        <v>315</v>
+        <v>290</v>
       </c>
     </row>
     <row r="409" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A409" s="5" t="s">
-        <v>316</v>
+        <v>291</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A410" s="6" t="s">
-        <v>317</v>
+        <v>292</v>
       </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411" s="6" t="s">
-        <v>318</v>
+        <v>612</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A412" s="6" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A413" s="6" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A414" s="6" t="s">
-        <v>320</v>
+        <v>294</v>
       </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A415" s="6" t="s">
-        <v>321</v>
+        <v>295</v>
       </c>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A416" s="6" t="s">
-        <v>322</v>
+        <v>296</v>
       </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A417" s="6" t="s">
-        <v>323</v>
+        <v>297</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A418" s="6" t="s">
-        <v>516</v>
+        <v>483</v>
       </c>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A419" s="6" t="s">
-        <v>517</v>
+        <v>484</v>
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A420" s="6" t="s">
-        <v>324</v>
+        <v>298</v>
       </c>
     </row>
     <row r="421" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A421" s="5" t="s">
-        <v>325</v>
+        <v>299</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A422" s="6" t="s">
-        <v>326</v>
+        <v>300</v>
       </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A423" s="6" t="s">
-        <v>327</v>
+        <v>301</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A424" s="6" t="s">
-        <v>328</v>
+        <v>302</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A425" s="6" t="s">
-        <v>329</v>
+        <v>303</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A426" s="6" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A427" s="6" t="s">
-        <v>331</v>
+        <v>305</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A428" s="6" t="s">
-        <v>332</v>
+        <v>306</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A429" s="6" t="s">
-        <v>333</v>
+        <v>307</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A430" s="6" t="s">
-        <v>334</v>
+        <v>308</v>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A431" s="6" t="s">
-        <v>335</v>
+        <v>309</v>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A432" s="6" t="s">
-        <v>519</v>
+        <v>486</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A433" s="6" t="s">
-        <v>518</v>
+        <v>485</v>
       </c>
     </row>
     <row r="434" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A434" s="5" t="s">
-        <v>336</v>
+        <v>310</v>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A435" s="6" t="s">
-        <v>337</v>
+        <v>311</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A436" s="6" t="s">
-        <v>338</v>
+        <v>312</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A437" s="6" t="s">
-        <v>339</v>
+        <v>313</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A438" s="6" t="s">
-        <v>340</v>
+        <v>314</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A439" s="6" t="s">
-        <v>341</v>
+        <v>315</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A440" s="6" t="s">
-        <v>342</v>
+        <v>316</v>
       </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A441" s="6" t="s">
-        <v>343</v>
+        <v>317</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A442" s="6" t="s">
-        <v>344</v>
+        <v>318</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A443" s="6" t="s">
-        <v>345</v>
+        <v>319</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A444" s="6" t="s">
-        <v>346</v>
+        <v>320</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A445" s="6" t="s">
-        <v>520</v>
+        <v>487</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A446" s="6" t="s">
-        <v>521</v>
+        <v>488</v>
       </c>
     </row>
     <row r="447" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A447" s="5" t="s">
-        <v>347</v>
+        <v>321</v>
       </c>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A448" s="6" t="s">
-        <v>348</v>
+        <v>635</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A449" s="6" t="s">
-        <v>349</v>
+        <v>322</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A450" s="6" t="s">
-        <v>350</v>
+        <v>323</v>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A451" s="6" t="s">
-        <v>351</v>
+        <v>324</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A452" s="6" t="s">
-        <v>352</v>
+        <v>325</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A453" s="6" t="s">
-        <v>522</v>
+        <v>489</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A454" s="6" t="s">
-        <v>353</v>
+        <v>326</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A455" s="6" t="s">
-        <v>354</v>
+        <v>636</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A456" s="6" t="s">
-        <v>355</v>
+        <v>327</v>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A457" s="6" t="s">
-        <v>356</v>
+        <v>328</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A458" s="6" t="s">
-        <v>523</v>
+        <v>490</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A459" s="6" t="s">
-        <v>557</v>
+        <v>520</v>
       </c>
     </row>
     <row r="460" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A460" s="5" t="s">
-        <v>357</v>
+        <v>329</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A461" s="6" t="s">
-        <v>358</v>
+        <v>330</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A462" s="6" t="s">
-        <v>359</v>
+        <v>331</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A463" s="6" t="s">
-        <v>360</v>
+        <v>332</v>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A464" s="6" t="s">
-        <v>361</v>
+        <v>333</v>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A465" s="6" t="s">
-        <v>362</v>
+        <v>334</v>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A466" s="6" t="s">
-        <v>363</v>
+        <v>335</v>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A467" s="6" t="s">
-        <v>364</v>
+        <v>336</v>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A468" s="6" t="s">
-        <v>365</v>
+        <v>337</v>
       </c>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A469" s="6" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A470" s="6" t="s">
-        <v>367</v>
+        <v>339</v>
       </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A471" s="6" t="s">
-        <v>524</v>
+        <v>491</v>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A472" s="6" t="s">
-        <v>525</v>
+        <v>492</v>
       </c>
     </row>
     <row r="473" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A473" s="5" t="s">
-        <v>368</v>
+        <v>340</v>
       </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A474" s="6" t="s">
-        <v>369</v>
+        <v>341</v>
       </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A475" s="6" t="s">
-        <v>370</v>
+        <v>342</v>
       </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A476" s="6" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A477" s="6" t="s">
-        <v>372</v>
+        <v>344</v>
       </c>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A478" s="6" t="s">
-        <v>373</v>
+        <v>345</v>
       </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A479" s="6" t="s">
-        <v>374</v>
+        <v>346</v>
       </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A480" s="6" t="s">
-        <v>375</v>
+        <v>637</v>
       </c>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A481" s="6" t="s">
-        <v>376</v>
+        <v>347</v>
       </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A482" s="6" t="s">
-        <v>377</v>
+        <v>638</v>
       </c>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A483" s="6" t="s">
-        <v>378</v>
+        <v>348</v>
       </c>
     </row>
     <row r="484" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A484" s="5" t="s">
-        <v>379</v>
+        <v>349</v>
       </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A485" s="6" t="s">
-        <v>380</v>
+        <v>350</v>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A486" s="6" t="s">
-        <v>381</v>
+        <v>351</v>
       </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A487" s="6" t="s">
-        <v>382</v>
+        <v>352</v>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A488" s="6" t="s">
-        <v>383</v>
+        <v>353</v>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A489" s="6" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A490" s="6" t="s">
-        <v>384</v>
+        <v>354</v>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A491" s="6" t="s">
-        <v>385</v>
+        <v>355</v>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A492" s="6" t="s">
-        <v>335</v>
+        <v>309</v>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A493" s="6" t="s">
-        <v>386</v>
+        <v>356</v>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A494" s="6" t="s">
-        <v>387</v>
+        <v>357</v>
       </c>
     </row>
     <row r="495" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A495" s="5" t="s">
-        <v>388</v>
+        <v>358</v>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A496" s="6" t="s">
-        <v>389</v>
+        <v>359</v>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A497" s="6" t="s">
-        <v>390</v>
+        <v>360</v>
       </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A498" s="6" t="s">
-        <v>391</v>
+        <v>361</v>
       </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A499" s="6" t="s">
-        <v>392</v>
+        <v>362</v>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A500" s="6" t="s">
-        <v>300</v>
+        <v>275</v>
       </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A501" s="6" t="s">
-        <v>393</v>
+        <v>363</v>
       </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A502" s="6" t="s">
-        <v>394</v>
+        <v>364</v>
       </c>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A503" s="6" t="s">
-        <v>395</v>
+        <v>365</v>
       </c>
     </row>
     <row r="504" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A504" s="5" t="s">
-        <v>396</v>
+        <v>366</v>
       </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A505" s="6" t="s">
-        <v>397</v>
+        <v>367</v>
       </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A506" s="6" t="s">
-        <v>526</v>
+        <v>493</v>
       </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A507" s="6" t="s">
-        <v>527</v>
+        <v>494</v>
       </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A508" s="6" t="s">
-        <v>398</v>
+        <v>368</v>
       </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A509" s="6" t="s">
-        <v>399</v>
+        <v>369</v>
       </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A510" s="6" t="s">
-        <v>400</v>
+        <v>370</v>
       </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A511" s="6" t="s">
-        <v>529</v>
+        <v>496</v>
       </c>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A512" s="6" t="s">
-        <v>530</v>
+        <v>497</v>
       </c>
     </row>
     <row r="513" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A513" s="7" t="s">
-        <v>528</v>
+        <v>495</v>
       </c>
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A514" s="6" t="s">
-        <v>401</v>
+        <v>371</v>
       </c>
     </row>
     <row r="515" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A515" s="6" t="s">
-        <v>402</v>
+        <v>372</v>
       </c>
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A516" s="6" t="s">
-        <v>403</v>
+        <v>373</v>
       </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A517" s="6" t="s">
-        <v>404</v>
+        <v>374</v>
       </c>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A518" s="6" t="s">
-        <v>531</v>
+        <v>498</v>
       </c>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A519" s="6" t="s">
-        <v>532</v>
+        <v>499</v>
       </c>
     </row>
     <row r="520" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A520" s="6" t="s">
-        <v>405</v>
+        <v>375</v>
       </c>
     </row>
     <row r="521" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A521" s="6" t="s">
-        <v>406</v>
+        <v>376</v>
       </c>
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A522" s="6" t="s">
-        <v>533</v>
+        <v>627</v>
       </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A523" s="6" t="s">
-        <v>558</v>
+        <v>521</v>
       </c>
     </row>
     <row r="524" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A524" s="5" t="s">
-        <v>407</v>
+        <v>377</v>
       </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A525" s="6" t="s">
-        <v>408</v>
+        <v>378</v>
       </c>
     </row>
     <row r="526" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A526" s="6" t="s">
-        <v>409</v>
+        <v>379</v>
       </c>
     </row>
     <row r="527" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A527" s="6" t="s">
-        <v>410</v>
+        <v>380</v>
       </c>
     </row>
     <row r="528" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A528" s="6" t="s">
-        <v>411</v>
+        <v>381</v>
       </c>
     </row>
     <row r="529" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A529" s="6" t="s">
-        <v>412</v>
+        <v>382</v>
       </c>
     </row>
     <row r="530" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A530" s="6" t="s">
-        <v>413</v>
+        <v>383</v>
       </c>
     </row>
     <row r="531" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A531" s="6" t="s">
-        <v>414</v>
+        <v>384</v>
       </c>
     </row>
     <row r="532" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A532" s="6" t="s">
-        <v>415</v>
+        <v>628</v>
       </c>
     </row>
     <row r="533" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A533" s="6" t="s">
-        <v>416</v>
+        <v>385</v>
       </c>
     </row>
     <row r="534" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A534" s="6" t="s">
-        <v>417</v>
+        <v>386</v>
       </c>
     </row>
     <row r="535" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A535" s="6" t="s">
-        <v>418</v>
+        <v>387</v>
       </c>
     </row>
     <row r="536" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A536" s="5" t="s">
-        <v>419</v>
+        <v>388</v>
       </c>
     </row>
     <row r="537" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A537" s="6" t="s">
-        <v>420</v>
+        <v>389</v>
       </c>
     </row>
     <row r="538" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A538" s="6" t="s">
-        <v>421</v>
+        <v>390</v>
       </c>
     </row>
     <row r="539" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A539" s="6" t="s">
-        <v>422</v>
+        <v>391</v>
       </c>
     </row>
     <row r="540" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A540" s="6" t="s">
-        <v>423</v>
+        <v>392</v>
       </c>
     </row>
     <row r="541" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A541" s="6" t="s">
-        <v>424</v>
+        <v>393</v>
       </c>
     </row>
     <row r="542" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A542" s="6" t="s">
-        <v>425</v>
+        <v>394</v>
       </c>
     </row>
     <row r="543" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A543" s="6" t="s">
-        <v>426</v>
+        <v>395</v>
       </c>
     </row>
     <row r="544" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A544" s="6" t="s">
-        <v>427</v>
+        <v>396</v>
       </c>
     </row>
     <row r="545" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A545" s="6" t="s">
-        <v>534</v>
+        <v>633</v>
       </c>
     </row>
     <row r="546" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A546" s="6" t="s">
-        <v>535</v>
+        <v>500</v>
       </c>
     </row>
     <row r="547" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A547" s="6" t="s">
-        <v>428</v>
+        <v>397</v>
       </c>
     </row>
     <row r="548" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A548" s="5" t="s">
-        <v>429</v>
+        <v>398</v>
       </c>
     </row>
     <row r="549" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A549" s="6" t="s">
-        <v>430</v>
+        <v>399</v>
       </c>
     </row>
     <row r="550" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A550" s="6" t="s">
-        <v>431</v>
+        <v>400</v>
       </c>
     </row>
     <row r="551" spans="1:4" ht="18" x14ac:dyDescent="0.3">
       <c r="A551" s="6" t="s">
-        <v>432</v>
+        <v>401</v>
       </c>
     </row>
     <row r="552" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A552" s="6" t="s">
-        <v>433</v>
+        <v>402</v>
       </c>
     </row>
     <row r="553" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A553" s="6" t="s">
-        <v>434</v>
+        <v>403</v>
       </c>
     </row>
     <row r="554" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A554" s="6" t="s">
-        <v>435</v>
+        <v>404</v>
       </c>
     </row>
     <row r="555" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A555" s="6" t="s">
-        <v>436</v>
+        <v>405</v>
       </c>
     </row>
     <row r="556" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A556" s="6" t="s">
-        <v>437</v>
+        <v>406</v>
       </c>
     </row>
     <row r="557" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A557" s="6" t="s">
-        <v>438</v>
+        <v>407</v>
       </c>
     </row>
     <row r="558" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A558" s="6" t="s">
-        <v>439</v>
+        <v>408</v>
       </c>
       <c r="D558" s="1"/>
     </row>
     <row r="559" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A559" s="5" t="s">
-        <v>440</v>
+        <v>409</v>
       </c>
       <c r="D559" s="1"/>
     </row>
     <row r="560" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A560" s="6" t="s">
-        <v>441</v>
+        <v>410</v>
       </c>
       <c r="D560" s="1"/>
     </row>
     <row r="561" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A561" s="6" t="s">
-        <v>442</v>
+        <v>411</v>
       </c>
       <c r="D561" s="1"/>
     </row>
     <row r="562" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A562" s="6" t="s">
-        <v>443</v>
+        <v>412</v>
       </c>
     </row>
     <row r="563" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A563" s="6" t="s">
-        <v>444</v>
+        <v>413</v>
       </c>
     </row>
     <row r="564" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A564" s="6" t="s">
-        <v>536</v>
+        <v>501</v>
       </c>
     </row>
     <row r="565" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A565" s="6" t="s">
-        <v>537</v>
+        <v>502</v>
       </c>
     </row>
     <row r="566" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A566" s="6" t="s">
-        <v>445</v>
+        <v>414</v>
       </c>
     </row>
     <row r="567" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A567" s="6" t="s">
-        <v>446</v>
+        <v>415</v>
       </c>
     </row>
     <row r="568" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A568" s="6" t="s">
-        <v>447</v>
+        <v>416</v>
       </c>
     </row>
     <row r="569" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A569" s="6" t="s">
-        <v>448</v>
+        <v>417</v>
       </c>
     </row>
     <row r="570" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A570" s="5" t="s">
-        <v>449</v>
+        <v>418</v>
       </c>
     </row>
     <row r="571" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A571" s="6" t="s">
-        <v>450</v>
+        <v>419</v>
       </c>
     </row>
     <row r="572" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A572" s="6" t="s">
-        <v>451</v>
+        <v>420</v>
       </c>
     </row>
     <row r="573" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A573" s="6" t="s">
-        <v>452</v>
+        <v>421</v>
       </c>
     </row>
     <row r="574" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A574" s="6" t="s">
-        <v>453</v>
+        <v>422</v>
       </c>
     </row>
     <row r="575" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A575" s="6" t="s">
-        <v>454</v>
+        <v>423</v>
       </c>
     </row>
     <row r="576" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A576" s="6" t="s">
-        <v>455</v>
+        <v>424</v>
       </c>
     </row>
     <row r="577" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A577" s="6" t="s">
-        <v>456</v>
+        <v>425</v>
       </c>
     </row>
     <row r="578" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A578" s="6" t="s">
-        <v>457</v>
+        <v>426</v>
       </c>
     </row>
     <row r="579" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A579" s="6" t="s">
-        <v>458</v>
+        <v>427</v>
       </c>
     </row>
     <row r="580" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A580" s="4" t="s">
-        <v>559</v>
+        <v>522</v>
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A581" s="3" t="s">
-        <v>560</v>
+        <v>523</v>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A582" s="4" t="s">
-        <v>561</v>
+        <v>524</v>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A583" s="4" t="s">
-        <v>562</v>
+        <v>525</v>
       </c>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A584" s="4" t="s">
-        <v>563</v>
+        <v>526</v>
       </c>
     </row>
     <row r="585" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A585" s="4" t="s">
-        <v>564</v>
+        <v>527</v>
       </c>
     </row>
     <row r="586" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A586" s="4" t="s">
-        <v>565</v>
+        <v>528</v>
       </c>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A587" s="4" t="s">
-        <v>584</v>
+        <v>546</v>
       </c>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A588" s="4" t="s">
-        <v>566</v>
+        <v>529</v>
       </c>
     </row>
     <row r="589" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A589" s="4" t="s">
-        <v>585</v>
+        <v>547</v>
       </c>
     </row>
     <row r="590" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A590" s="4" t="s">
-        <v>568</v>
+        <v>531</v>
       </c>
     </row>
     <row r="591" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A591" s="4" t="s">
-        <v>567</v>
+        <v>530</v>
       </c>
     </row>
     <row r="592" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A592" s="4" t="s">
-        <v>583</v>
+        <v>545</v>
       </c>
     </row>
     <row r="593" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A593" s="3" t="s">
-        <v>569</v>
+        <v>532</v>
       </c>
     </row>
     <row r="594" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A594" s="4" t="s">
-        <v>627</v>
+        <v>587</v>
       </c>
     </row>
     <row r="595" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A595" s="4" t="s">
-        <v>601</v>
+        <v>563</v>
       </c>
     </row>
     <row r="596" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A596" s="4" t="s">
-        <v>585</v>
+        <v>547</v>
       </c>
     </row>
     <row r="597" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A597" s="4" t="s">
-        <v>602</v>
+        <v>564</v>
       </c>
     </row>
     <row r="598" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A598" s="4" t="s">
-        <v>600</v>
+        <v>562</v>
       </c>
     </row>
     <row r="599" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A599" s="4" t="s">
-        <v>598</v>
+        <v>560</v>
       </c>
     </row>
     <row r="600" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A600" s="4" t="s">
-        <v>599</v>
+        <v>561</v>
       </c>
     </row>
     <row r="601" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A601" s="4" t="s">
-        <v>597</v>
+        <v>559</v>
       </c>
     </row>
     <row r="602" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A602" s="4" t="s">
-        <v>596</v>
+        <v>558</v>
       </c>
     </row>
     <row r="603" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A603" s="3" t="s">
-        <v>581</v>
+        <v>543</v>
       </c>
     </row>
     <row r="604" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A604" s="4" t="s">
-        <v>612</v>
+        <v>572</v>
       </c>
     </row>
     <row r="605" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A605" s="4" t="s">
-        <v>613</v>
+        <v>573</v>
       </c>
     </row>
     <row r="606" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A606" s="4" t="s">
-        <v>614</v>
+        <v>574</v>
       </c>
     </row>
     <row r="607" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A607" s="4" t="s">
-        <v>615</v>
+        <v>575</v>
       </c>
     </row>
     <row r="608" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A608" s="4" t="s">
-        <v>616</v>
+        <v>576</v>
       </c>
     </row>
     <row r="609" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A609" s="4" t="s">
-        <v>609</v>
+        <v>570</v>
       </c>
     </row>
     <row r="610" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A610" s="4" t="s">
-        <v>617</v>
+        <v>577</v>
       </c>
     </row>
     <row r="611" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A611" s="4" t="s">
-        <v>618</v>
+        <v>578</v>
       </c>
     </row>
     <row r="612" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A612" s="4" t="s">
-        <v>619</v>
+        <v>579</v>
       </c>
     </row>
     <row r="613" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A613" s="4" t="s">
-        <v>620</v>
+        <v>580</v>
       </c>
     </row>
     <row r="614" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A614" s="4" t="s">
-        <v>564</v>
+        <v>527</v>
       </c>
     </row>
     <row r="615" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A615" s="4" t="s">
-        <v>600</v>
+        <v>562</v>
       </c>
     </row>
     <row r="616" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A616" s="4" t="s">
-        <v>621</v>
+        <v>581</v>
       </c>
     </row>
     <row r="617" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A617" s="4" t="s">
-        <v>570</v>
+        <v>614</v>
       </c>
     </row>
     <row r="618" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A618" s="4" t="s">
-        <v>622</v>
+        <v>582</v>
       </c>
     </row>
     <row r="619" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A619" s="4" t="s">
-        <v>598</v>
+        <v>560</v>
       </c>
     </row>
     <row r="620" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A620" s="4" t="s">
-        <v>626</v>
+        <v>586</v>
       </c>
     </row>
     <row r="621" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A621" s="4" t="s">
-        <v>623</v>
+        <v>583</v>
       </c>
     </row>
     <row r="622" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A622" s="4" t="s">
-        <v>624</v>
+        <v>584</v>
       </c>
     </row>
     <row r="623" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A623" s="4" t="s">
-        <v>604</v>
+        <v>565</v>
       </c>
     </row>
     <row r="624" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A624" s="4" t="s">
-        <v>625</v>
+        <v>585</v>
       </c>
     </row>
     <row r="625" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A625" s="3" t="s">
-        <v>582</v>
+        <v>544</v>
       </c>
     </row>
     <row r="626" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A626" s="4" t="s">
-        <v>571</v>
+        <v>533</v>
       </c>
     </row>
     <row r="627" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A627" s="4" t="s">
-        <v>572</v>
+        <v>534</v>
       </c>
     </row>
     <row r="628" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A628" s="4" t="s">
-        <v>573</v>
+        <v>535</v>
       </c>
     </row>
     <row r="629" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A629" s="4" t="s">
-        <v>574</v>
+        <v>536</v>
       </c>
     </row>
     <row r="630" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A630" s="4" t="s">
-        <v>575</v>
+        <v>537</v>
       </c>
     </row>
     <row r="631" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A631" s="4" t="s">
-        <v>576</v>
+        <v>538</v>
       </c>
     </row>
     <row r="632" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A632" s="4" t="s">
-        <v>641</v>
+        <v>600</v>
       </c>
     </row>
     <row r="633" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A633" s="4" t="s">
-        <v>577</v>
+        <v>539</v>
       </c>
     </row>
     <row r="634" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A634" s="4" t="s">
-        <v>578</v>
+        <v>540</v>
       </c>
     </row>
     <row r="635" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A635" s="4" t="s">
-        <v>579</v>
+        <v>541</v>
       </c>
     </row>
     <row r="636" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A636" s="4" t="s">
-        <v>580</v>
+        <v>542</v>
       </c>
     </row>
     <row r="637" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A637" s="3" t="s">
-        <v>611</v>
+        <v>571</v>
       </c>
     </row>
     <row r="638" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A638" s="4" t="s">
-        <v>571</v>
+        <v>533</v>
       </c>
     </row>
     <row r="639" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A639" s="4" t="s">
-        <v>587</v>
+        <v>549</v>
       </c>
     </row>
     <row r="640" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A640" s="4" t="s">
-        <v>588</v>
+        <v>550</v>
       </c>
     </row>
     <row r="641" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A641" s="4" t="s">
-        <v>586</v>
+        <v>548</v>
       </c>
     </row>
     <row r="642" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A642" s="4" t="s">
-        <v>589</v>
+        <v>551</v>
       </c>
     </row>
     <row r="643" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A643" s="4" t="s">
-        <v>590</v>
+        <v>552</v>
       </c>
     </row>
     <row r="644" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A644" s="4" t="s">
-        <v>591</v>
+        <v>553</v>
       </c>
     </row>
     <row r="645" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A645" s="4" t="s">
-        <v>592</v>
+        <v>554</v>
       </c>
     </row>
     <row r="646" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A646" s="4" t="s">
-        <v>593</v>
+        <v>555</v>
       </c>
     </row>
     <row r="647" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A647" s="4" t="s">
-        <v>594</v>
+        <v>556</v>
       </c>
     </row>
     <row r="648" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A648" s="4" t="s">
-        <v>595</v>
+        <v>557</v>
       </c>
     </row>
     <row r="649" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A649" s="3" t="s">
-        <v>636</v>
+        <v>595</v>
       </c>
     </row>
     <row r="650" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A650" s="4" t="s">
-        <v>570</v>
+        <v>614</v>
       </c>
     </row>
     <row r="651" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A651" s="4" t="s">
-        <v>605</v>
+        <v>566</v>
       </c>
     </row>
     <row r="652" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A652" s="4" t="s">
-        <v>606</v>
+        <v>567</v>
       </c>
     </row>
     <row r="653" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A653" s="4" t="s">
-        <v>607</v>
+        <v>568</v>
       </c>
     </row>
     <row r="654" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A654" s="4" t="s">
-        <v>609</v>
+        <v>570</v>
       </c>
     </row>
     <row r="655" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A655" s="4" t="s">
-        <v>603</v>
+        <v>640</v>
       </c>
     </row>
     <row r="656" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A656" s="4" t="s">
-        <v>604</v>
+        <v>565</v>
       </c>
     </row>
     <row r="657" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A657" s="4" t="s">
-        <v>640</v>
+        <v>599</v>
       </c>
     </row>
     <row r="658" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A658" s="4" t="s">
-        <v>608</v>
+        <v>569</v>
       </c>
     </row>
     <row r="659" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A659" s="4" t="s">
-        <v>610</v>
+        <v>639</v>
       </c>
     </row>
     <row r="660" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A660" s="3" t="s">
-        <v>637</v>
+        <v>596</v>
       </c>
     </row>
     <row r="661" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A661" s="4" t="s">
-        <v>628</v>
+        <v>613</v>
       </c>
     </row>
     <row r="662" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A662" s="4" t="s">
-        <v>629</v>
+        <v>588</v>
       </c>
     </row>
     <row r="663" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A663" s="4" t="s">
-        <v>630</v>
+        <v>589</v>
       </c>
     </row>
     <row r="664" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A664" s="4" t="s">
-        <v>631</v>
+        <v>590</v>
       </c>
     </row>
     <row r="665" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A665" s="4" t="s">
-        <v>632</v>
+        <v>591</v>
       </c>
     </row>
     <row r="666" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A666" s="4" t="s">
-        <v>633</v>
+        <v>592</v>
       </c>
     </row>
     <row r="667" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A667" s="4" t="s">
-        <v>635</v>
+        <v>594</v>
       </c>
     </row>
     <row r="668" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A668" s="4" t="s">
-        <v>634</v>
+        <v>593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>